<commit_message>
Add some keys for arguments in receptionist scenario
</commit_message>
<xml_diff>
--- a/global.xlsx
+++ b/global.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\robocup\data-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A784066A-B176-4001-B3E0-6F4B1B88DF7D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1F8E5C-77A2-4458-8564-E80F6B34A840}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>Bin</t>
   </si>
@@ -169,6 +169,18 @@
   </si>
   <si>
     <t>Keys in JSON</t>
+  </si>
+  <si>
+    <t>img/location/bar.png</t>
+  </si>
+  <si>
+    <t>img/location/livingRoom.png</t>
+  </si>
+  <si>
+    <t>img/location/entrance.png</t>
+  </si>
+  <si>
+    <t>img/location/bin.png</t>
   </si>
 </sst>
 </file>
@@ -636,68 +648,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29262BD-60A5-4908-8695-58186B5D3D51}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="40.7109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>0</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C3" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C4" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>2</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C5" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>3</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>0</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -711,7 +743,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -873,7 +905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90534E3A-7880-491D-A8C4-E1DCE011873C}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Change locations's id by string instead of number
</commit_message>
<xml_diff>
--- a/global.xlsx
+++ b/global.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\robocup\data-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1F8E5C-77A2-4458-8564-E80F6B34A840}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C57680-530C-4CDA-9277-70B97590A339}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3555" yWindow="3045" windowWidth="21600" windowHeight="7200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
   <si>
     <t>Bin</t>
   </si>
@@ -181,6 +181,18 @@
   </si>
   <si>
     <t>img/location/bin.png</t>
+  </si>
+  <si>
+    <t>bar</t>
+  </si>
+  <si>
+    <t>livingRoom</t>
+  </si>
+  <si>
+    <t>entrance</t>
+  </si>
+  <si>
+    <t>bin</t>
   </si>
 </sst>
 </file>
@@ -650,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29262BD-60A5-4908-8695-58186B5D3D51}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -689,8 +701,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
-        <v>0</v>
+      <c r="A3" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>3</v>
@@ -700,8 +712,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
-        <v>1</v>
+      <c r="A4" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>2</v>
@@ -711,8 +723,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
-        <v>2</v>
+      <c r="A5" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>1</v>
@@ -722,8 +734,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
-        <v>3</v>
+      <c r="A6" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Fix script to python3, automatically remove trailling spaces
</commit_message>
<xml_diff>
--- a/global.xlsx
+++ b/global.xlsx
@@ -1,29 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21722"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\robocup\data-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C57680-530C-4CDA-9277-70B97590A339}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D009A50-5CF3-48EB-8FA6-1DC43F185583}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="3045" windowWidth="21600" windowHeight="7200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="2" r:id="rId1"/>
     <sheet name="Drinks" sheetId="3" r:id="rId2"/>
-    <sheet name="People" sheetId="4" r:id="rId3"/>
+    <sheet name="Variables" sheetId="5" r:id="rId3"/>
+    <sheet name="People" sheetId="4" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
+    <definedName name="female">People!$E$3</definedName>
     <definedName name="guest1">[1]Meta!$B$7</definedName>
     <definedName name="guest2">[1]Meta!$B$8</definedName>
     <definedName name="KnownPerson">[1]Meta!$B$6</definedName>
+    <definedName name="male">People!$E$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="75">
   <si>
     <t>Bin</t>
   </si>
@@ -126,33 +129,6 @@
     <t>Drinks</t>
   </si>
   <si>
-    <t>Neo</t>
-  </si>
-  <si>
-    <t>Bill</t>
-  </si>
-  <si>
-    <t>Sally</t>
-  </si>
-  <si>
-    <t>Matt</t>
-  </si>
-  <si>
-    <t>Clara</t>
-  </si>
-  <si>
-    <t>Jack</t>
-  </si>
-  <si>
-    <t>Rose</t>
-  </si>
-  <si>
-    <t>Rory</t>
-  </si>
-  <si>
-    <t>Amy</t>
-  </si>
-  <si>
     <t>John</t>
   </si>
   <si>
@@ -193,6 +169,105 @@
   </si>
   <si>
     <t>bin</t>
+  </si>
+  <si>
+    <t>Location (ALMemory)</t>
+  </si>
+  <si>
+    <t>Key 1</t>
+  </si>
+  <si>
+    <t>Value 1</t>
+  </si>
+  <si>
+    <t>Key 2</t>
+  </si>
+  <si>
+    <t>Value 2</t>
+  </si>
+  <si>
+    <t>Key 3</t>
+  </si>
+  <si>
+    <t>Value 3</t>
+  </si>
+  <si>
+    <t>guest</t>
+  </si>
+  <si>
+    <t>drinkId</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Richard</t>
+  </si>
+  <si>
+    <t>Charles</t>
+  </si>
+  <si>
+    <t>Joseph</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Sophia</t>
+  </si>
+  <si>
+    <t>Isabella</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>Olivia</t>
+  </si>
+  <si>
+    <t>Ava</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Abigail</t>
+  </si>
+  <si>
+    <t>Madison</t>
+  </si>
+  <si>
+    <t>Mia</t>
+  </si>
+  <si>
+    <t>Chloe</t>
+  </si>
+  <si>
+    <t>Gender list</t>
   </si>
 </sst>
 </file>
@@ -320,7 +395,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -342,6 +417,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
@@ -662,13 +746,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29262BD-60A5-4908-8695-58186B5D3D51}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.7109375" style="1" customWidth="1"/>
     <col min="4" max="5" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -688,60 +772,60 @@
     </row>
     <row r="2" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -755,7 +839,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A2" sqref="A2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -770,7 +854,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>27</v>
@@ -781,16 +865,16 @@
     </row>
     <row r="2" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -914,84 +998,305 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D19B18E-5623-4DC4-818D-50C0A41569B3}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="13"/>
+    <col min="4" max="4" width="10.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="11">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90534E3A-7880-491D-A8C4-E1DCE011873C}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="B3" s="7" t="str">
+        <f>female</f>
+        <v>female</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="B4" s="7" t="str">
+        <f>female</f>
+        <v>female</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="B5" s="7" t="str">
+        <f>female</f>
+        <v>female</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="B6" s="7" t="str">
+        <f>female</f>
+        <v>female</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="B7" s="7" t="str">
+        <f>female</f>
+        <v>female</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="B8" s="7" t="str">
+        <f>female</f>
+        <v>female</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="B9" s="7" t="str">
+        <f>female</f>
+        <v>female</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="B10" s="7" t="str">
+        <f>female</f>
+        <v>female</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="B11" s="7" t="str">
+        <f>female</f>
+        <v>female</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="7" t="str">
+        <f>female</f>
+        <v>female</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="7" t="str">
+        <f>male</f>
+        <v>male</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>28</v>
+      </c>
+      <c r="B14" s="7" t="str">
+        <f>male</f>
+        <v>male</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="7" t="str">
+        <f>male</f>
+        <v>male</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="7" t="str">
+        <f>male</f>
+        <v>male</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="7" t="str">
+        <f>male</f>
+        <v>male</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="7" t="str">
+        <f>male</f>
+        <v>male</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="7" t="str">
+        <f>male</f>
+        <v>male</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="7" t="str">
+        <f>male</f>
+        <v>male</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="7" t="str">
+        <f>male</f>
+        <v>male</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="7" t="str">
+        <f>male</f>
+        <v>male</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>

</xml_diff>